<commit_message>
Got CLR and OLR into shape to attempt (hopefully final) test ingest
</commit_message>
<xml_diff>
--- a/course_catalogs/OLR/xls_standard_input_UCSD-course-catalogs.xlsx
+++ b/course_catalogs/OLR/xls_standard_input_UCSD-course-catalogs.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\UCSD-course-catalogs\Final_metadata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\domm-metadata\course_catalogs\OLR\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23790" windowHeight="11835" tabRatio="418"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23790" windowHeight="9630" tabRatio="377"/>
   </bookViews>
   <sheets>
     <sheet name="Item description" sheetId="9" r:id="rId1"/>
@@ -26,7 +26,7 @@
     <author>Windows User</author>
   </authors>
   <commentList>
-    <comment ref="I1" authorId="0" shapeId="0">
+    <comment ref="K1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -58,7 +58,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0" shapeId="0">
+    <comment ref="L1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -93,7 +93,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0" shapeId="0">
+    <comment ref="M1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -133,7 +133,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1136" uniqueCount="895">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1228" uniqueCount="941">
   <si>
     <t>text</t>
   </si>
@@ -2818,6 +2818,144 @@
   </si>
   <si>
     <t>This catalog is for all colleges.</t>
+  </si>
+  <si>
+    <t>File use 2</t>
+  </si>
+  <si>
+    <t>File name 2</t>
+  </si>
+  <si>
+    <t>UCSDGC_1991-1992.zip</t>
+  </si>
+  <si>
+    <t>UCSDGC_1992-1993.zip</t>
+  </si>
+  <si>
+    <t>UCSDGC_1982-1983.zip</t>
+  </si>
+  <si>
+    <t>UCSDGC_1983-1984.zip</t>
+  </si>
+  <si>
+    <t>UCSDGC_1981-1982.zip</t>
+  </si>
+  <si>
+    <t>UCSDGC_2002-2003.zip</t>
+  </si>
+  <si>
+    <t>UCSDGC_2003-2004.zip</t>
+  </si>
+  <si>
+    <t>UCSDGC_2004_2005.zip</t>
+  </si>
+  <si>
+    <t>UCSDGC_1971-1972.zip</t>
+  </si>
+  <si>
+    <t>UCSDGC_1972-1973.zip</t>
+  </si>
+  <si>
+    <t>UCSDGC_1974-1975.zip</t>
+  </si>
+  <si>
+    <t>UCSDGC_1973-1974.zip</t>
+  </si>
+  <si>
+    <t>UCSDGC_1967-1968.zip</t>
+  </si>
+  <si>
+    <t>UCSDGC_1961-1962.zip</t>
+  </si>
+  <si>
+    <t>UCSDGC_1966-1967.zip</t>
+  </si>
+  <si>
+    <t>UCSDGC_1965-1966.zip</t>
+  </si>
+  <si>
+    <t>UCSDGC_1963-1964.zip</t>
+  </si>
+  <si>
+    <t>UCSDGC_1966-1967_2.zip</t>
+  </si>
+  <si>
+    <t>UCSDGC_1962-1963.zip</t>
+  </si>
+  <si>
+    <t>UCSDGC_1964-1965.zip</t>
+  </si>
+  <si>
+    <t>UCSDGC_1968_1969.zip</t>
+  </si>
+  <si>
+    <t>UCSDGC_1970_1971.zip</t>
+  </si>
+  <si>
+    <t>UCSDGC_1969_1970.zip</t>
+  </si>
+  <si>
+    <t>UCSDGC_1998_1999.zip</t>
+  </si>
+  <si>
+    <t>UCSDGC_1979-1980.zip</t>
+  </si>
+  <si>
+    <t>UCSDGC_1978-1979.zip</t>
+  </si>
+  <si>
+    <t>UCSDGC_1980-1981.zip</t>
+  </si>
+  <si>
+    <t>UCSDGC_1996-1997.zip</t>
+  </si>
+  <si>
+    <t>UCSDGC_1987_1988.zip</t>
+  </si>
+  <si>
+    <t>UCSDGC_1988_1989.zip</t>
+  </si>
+  <si>
+    <t>UCSDGC_2005-2006.zip</t>
+  </si>
+  <si>
+    <t>UCSDGC_1985_1986.zip</t>
+  </si>
+  <si>
+    <t>UCSDGC_1984_1985.zip</t>
+  </si>
+  <si>
+    <t>UCSDGC_1986_1987.zip</t>
+  </si>
+  <si>
+    <t>UCSDGC_1977-1978.zip</t>
+  </si>
+  <si>
+    <t>UCSDGC_1994_1995.zip</t>
+  </si>
+  <si>
+    <t>UCSDGC_1993_1994.zip</t>
+  </si>
+  <si>
+    <t>UCSDGC_1975-1976.zip</t>
+  </si>
+  <si>
+    <t>UCSDGC_1976-1977.zip</t>
+  </si>
+  <si>
+    <t>UCSDGC_1999_2000.zip</t>
+  </si>
+  <si>
+    <t>UCSDGC_1995-1996.zip</t>
+  </si>
+  <si>
+    <t>UCSDGC_2000_2001.zip</t>
+  </si>
+  <si>
+    <t>UCSDGC_2006_2007.zip</t>
+  </si>
+  <si>
+    <t>UCSDGC_1990-1991.zip</t>
   </si>
 </sst>
 </file>
@@ -3890,10 +4028,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L46"/>
+  <dimension ref="A1:N46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3902,17 +4040,19 @@
     <col min="2" max="2" width="23.5703125" style="3" customWidth="1"/>
     <col min="3" max="3" width="44" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.7109375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22" style="3" customWidth="1"/>
-    <col min="7" max="7" width="51.5703125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="45.140625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.85546875" style="3" customWidth="1"/>
-    <col min="11" max="11" width="15.140625" style="3" customWidth="1"/>
-    <col min="12" max="12" width="44" style="3" customWidth="1"/>
+    <col min="5" max="5" width="44" style="3" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" style="3" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22" style="3" customWidth="1"/>
+    <col min="9" max="9" width="51.5703125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="45.140625" style="3" customWidth="1"/>
+    <col min="11" max="11" width="13.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.85546875" style="3" customWidth="1"/>
+    <col min="13" max="13" width="15.140625" style="3" customWidth="1"/>
+    <col min="14" max="14" width="44" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>338</v>
       </c>
@@ -3926,31 +4066,37 @@
         <v>3</v>
       </c>
       <c r="E1" s="15" t="s">
+        <v>896</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>895</v>
+      </c>
+      <c r="G1" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="H1" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="I1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="J1" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="K1" s="16" t="s">
         <v>487</v>
       </c>
-      <c r="J1" s="16" t="s">
+      <c r="L1" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="16" t="s">
+      <c r="M1" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="15" t="s">
+      <c r="N1" s="15" t="s">
         <v>484</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>630</v>
       </c>
@@ -3963,30 +4109,36 @@
       <c r="D2" s="3" t="s">
         <v>384</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="23" t="s">
+        <v>897</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>358</v>
       </c>
-      <c r="G2" s="22" t="s">
+      <c r="I2" s="22" t="s">
         <v>719</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>761</v>
       </c>
-      <c r="I2" s="22" t="s">
+      <c r="K2" s="22" t="s">
         <v>762</v>
       </c>
-      <c r="J2" s="22" t="s">
+      <c r="L2" s="22" t="s">
         <v>805</v>
       </c>
-      <c r="K2" s="22" t="s">
+      <c r="M2" s="22" t="s">
         <v>848</v>
       </c>
-      <c r="L2" s="23"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N2" s="23"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>675</v>
       </c>
@@ -3999,30 +4151,36 @@
       <c r="D3" s="3" t="s">
         <v>384</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="23" t="s">
+        <v>898</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>358</v>
       </c>
-      <c r="G3" s="22" t="s">
+      <c r="I3" s="22" t="s">
         <v>720</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="J3" s="3" t="s">
         <v>761</v>
       </c>
-      <c r="I3" s="22" t="s">
+      <c r="K3" s="22" t="s">
         <v>763</v>
       </c>
-      <c r="J3" s="22" t="s">
+      <c r="L3" s="22" t="s">
         <v>806</v>
       </c>
-      <c r="K3" s="22" t="s">
+      <c r="M3" s="22" t="s">
         <v>849</v>
       </c>
-      <c r="L3" s="23"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N3" s="23"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>676</v>
       </c>
@@ -4035,30 +4193,36 @@
       <c r="D4" s="3" t="s">
         <v>384</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="23" t="s">
+        <v>899</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>358</v>
       </c>
-      <c r="G4" s="22" t="s">
+      <c r="I4" s="22" t="s">
         <v>721</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="J4" s="3" t="s">
         <v>761</v>
       </c>
-      <c r="I4" s="22" t="s">
+      <c r="K4" s="22" t="s">
         <v>764</v>
       </c>
-      <c r="J4" s="22" t="s">
+      <c r="L4" s="22" t="s">
         <v>807</v>
       </c>
-      <c r="K4" s="22" t="s">
+      <c r="M4" s="22" t="s">
         <v>850</v>
       </c>
-      <c r="L4" s="23"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N4" s="23"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>677</v>
       </c>
@@ -4071,30 +4235,36 @@
       <c r="D5" s="3" t="s">
         <v>384</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="23" t="s">
+        <v>900</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="G5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="H5" s="3" t="s">
         <v>358</v>
       </c>
-      <c r="G5" s="22" t="s">
+      <c r="I5" s="22" t="s">
         <v>722</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="J5" s="3" t="s">
         <v>761</v>
       </c>
-      <c r="I5" s="22" t="s">
+      <c r="K5" s="22" t="s">
         <v>765</v>
       </c>
-      <c r="J5" s="22" t="s">
+      <c r="L5" s="22" t="s">
         <v>808</v>
       </c>
-      <c r="K5" s="22" t="s">
+      <c r="M5" s="22" t="s">
         <v>851</v>
       </c>
-      <c r="L5" s="23"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N5" s="23"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>678</v>
       </c>
@@ -4107,30 +4277,36 @@
       <c r="D6" s="3" t="s">
         <v>384</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="23" t="s">
+        <v>901</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="H6" s="3" t="s">
         <v>358</v>
       </c>
-      <c r="G6" s="22" t="s">
+      <c r="I6" s="22" t="s">
         <v>723</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="J6" s="3" t="s">
         <v>761</v>
       </c>
-      <c r="I6" s="22" t="s">
+      <c r="K6" s="22" t="s">
         <v>766</v>
       </c>
-      <c r="J6" s="22" t="s">
+      <c r="L6" s="22" t="s">
         <v>809</v>
       </c>
-      <c r="K6" s="22" t="s">
+      <c r="M6" s="22" t="s">
         <v>852</v>
       </c>
-      <c r="L6" s="23"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N6" s="23"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>679</v>
       </c>
@@ -4143,30 +4319,36 @@
       <c r="D7" s="3" t="s">
         <v>384</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="23" t="s">
+        <v>902</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="G7" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="H7" s="3" t="s">
         <v>358</v>
       </c>
-      <c r="G7" s="22" t="s">
+      <c r="I7" s="22" t="s">
         <v>724</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="J7" s="3" t="s">
         <v>761</v>
       </c>
-      <c r="I7" s="22" t="s">
+      <c r="K7" s="22" t="s">
         <v>767</v>
       </c>
-      <c r="J7" s="22" t="s">
+      <c r="L7" s="22" t="s">
         <v>810</v>
       </c>
-      <c r="K7" s="22" t="s">
+      <c r="M7" s="22" t="s">
         <v>853</v>
       </c>
-      <c r="L7" s="23"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N7" s="23"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>680</v>
       </c>
@@ -4179,30 +4361,36 @@
       <c r="D8" s="3" t="s">
         <v>384</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="23" t="s">
+        <v>903</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="G8" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="H8" s="3" t="s">
         <v>358</v>
       </c>
-      <c r="G8" s="22" t="s">
+      <c r="I8" s="22" t="s">
         <v>725</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="J8" s="3" t="s">
         <v>761</v>
       </c>
-      <c r="I8" s="22" t="s">
+      <c r="K8" s="22" t="s">
         <v>768</v>
       </c>
-      <c r="J8" s="22" t="s">
+      <c r="L8" s="22" t="s">
         <v>811</v>
       </c>
-      <c r="K8" s="22" t="s">
+      <c r="M8" s="22" t="s">
         <v>854</v>
       </c>
-      <c r="L8" s="23"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N8" s="23"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>681</v>
       </c>
@@ -4215,30 +4403,36 @@
       <c r="D9" s="3" t="s">
         <v>384</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="23" t="s">
+        <v>904</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="G9" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="H9" s="3" t="s">
         <v>358</v>
       </c>
-      <c r="G9" s="22" t="s">
+      <c r="I9" s="22" t="s">
         <v>746</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="J9" s="3" t="s">
         <v>761</v>
       </c>
-      <c r="I9" s="22" t="s">
+      <c r="K9" s="22" t="s">
         <v>769</v>
       </c>
-      <c r="J9" s="22" t="s">
+      <c r="L9" s="22" t="s">
         <v>812</v>
       </c>
-      <c r="K9" s="22" t="s">
+      <c r="M9" s="22" t="s">
         <v>855</v>
       </c>
-      <c r="L9" s="23"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N9" s="23"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>682</v>
       </c>
@@ -4251,30 +4445,36 @@
       <c r="D10" s="3" t="s">
         <v>384</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="23" t="s">
+        <v>905</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="G10" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="H10" s="3" t="s">
         <v>358</v>
       </c>
-      <c r="G10" s="22" t="s">
+      <c r="I10" s="22" t="s">
         <v>726</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="J10" s="3" t="s">
         <v>761</v>
       </c>
-      <c r="I10" s="22" t="s">
+      <c r="K10" s="22" t="s">
         <v>770</v>
       </c>
-      <c r="J10" s="22" t="s">
+      <c r="L10" s="22" t="s">
         <v>813</v>
       </c>
-      <c r="K10" s="22" t="s">
+      <c r="M10" s="22" t="s">
         <v>856</v>
       </c>
-      <c r="L10" s="23"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N10" s="23"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>683</v>
       </c>
@@ -4287,30 +4487,36 @@
       <c r="D11" s="3" t="s">
         <v>384</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E11" s="23" t="s">
+        <v>906</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="G11" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="H11" s="3" t="s">
         <v>358</v>
       </c>
-      <c r="G11" s="22" t="s">
+      <c r="I11" s="22" t="s">
         <v>727</v>
       </c>
-      <c r="H11" s="3" t="s">
+      <c r="J11" s="3" t="s">
         <v>761</v>
       </c>
-      <c r="I11" s="22" t="s">
+      <c r="K11" s="22" t="s">
         <v>771</v>
       </c>
-      <c r="J11" s="22" t="s">
+      <c r="L11" s="22" t="s">
         <v>814</v>
       </c>
-      <c r="K11" s="22" t="s">
+      <c r="M11" s="22" t="s">
         <v>857</v>
       </c>
-      <c r="L11" s="23"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N11" s="23"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>684</v>
       </c>
@@ -4323,30 +4529,36 @@
       <c r="D12" s="3" t="s">
         <v>384</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" s="23" t="s">
+        <v>907</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="G12" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="H12" s="3" t="s">
         <v>358</v>
       </c>
-      <c r="G12" s="22" t="s">
+      <c r="I12" s="22" t="s">
         <v>728</v>
       </c>
-      <c r="H12" s="3" t="s">
+      <c r="J12" s="3" t="s">
         <v>761</v>
       </c>
-      <c r="I12" s="22" t="s">
+      <c r="K12" s="22" t="s">
         <v>772</v>
       </c>
-      <c r="J12" s="22" t="s">
+      <c r="L12" s="22" t="s">
         <v>815</v>
       </c>
-      <c r="K12" s="22" t="s">
+      <c r="M12" s="22" t="s">
         <v>858</v>
       </c>
-      <c r="L12" s="23"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N12" s="23"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>685</v>
       </c>
@@ -4359,30 +4571,36 @@
       <c r="D13" s="3" t="s">
         <v>384</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E13" s="23" t="s">
+        <v>908</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="G13" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="H13" s="3" t="s">
         <v>358</v>
       </c>
-      <c r="G13" s="22" t="s">
+      <c r="I13" s="22" t="s">
         <v>729</v>
       </c>
-      <c r="H13" s="3" t="s">
+      <c r="J13" s="3" t="s">
         <v>761</v>
       </c>
-      <c r="I13" s="22" t="s">
+      <c r="K13" s="22" t="s">
         <v>773</v>
       </c>
-      <c r="J13" s="22" t="s">
+      <c r="L13" s="22" t="s">
         <v>816</v>
       </c>
-      <c r="K13" s="22" t="s">
+      <c r="M13" s="22" t="s">
         <v>859</v>
       </c>
-      <c r="L13" s="23"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N13" s="23"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>686</v>
       </c>
@@ -4395,30 +4613,36 @@
       <c r="D14" s="3" t="s">
         <v>384</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="E14" s="23" t="s">
+        <v>909</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="G14" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="H14" s="3" t="s">
         <v>358</v>
       </c>
-      <c r="G14" s="22" t="s">
+      <c r="I14" s="22" t="s">
         <v>730</v>
       </c>
-      <c r="H14" s="3" t="s">
+      <c r="J14" s="3" t="s">
         <v>761</v>
       </c>
-      <c r="I14" s="22" t="s">
+      <c r="K14" s="22" t="s">
         <v>774</v>
       </c>
-      <c r="J14" s="22" t="s">
+      <c r="L14" s="22" t="s">
         <v>817</v>
       </c>
-      <c r="K14" s="22" t="s">
+      <c r="M14" s="22" t="s">
         <v>860</v>
       </c>
-      <c r="L14" s="23"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N14" s="23"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>687</v>
       </c>
@@ -4431,30 +4655,36 @@
       <c r="D15" s="3" t="s">
         <v>384</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="E15" s="23" t="s">
+        <v>910</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="G15" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="H15" s="3" t="s">
         <v>358</v>
       </c>
-      <c r="G15" s="22" t="s">
+      <c r="I15" s="22" t="s">
         <v>731</v>
       </c>
-      <c r="H15" s="3" t="s">
+      <c r="J15" s="3" t="s">
         <v>761</v>
       </c>
-      <c r="I15" s="22" t="s">
+      <c r="K15" s="22" t="s">
         <v>775</v>
       </c>
-      <c r="J15" s="22" t="s">
+      <c r="L15" s="22" t="s">
         <v>818</v>
       </c>
-      <c r="K15" s="22" t="s">
+      <c r="M15" s="22" t="s">
         <v>861</v>
       </c>
-      <c r="L15" s="23"/>
-    </row>
-    <row r="16" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="N15" s="23"/>
+    </row>
+    <row r="16" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>688</v>
       </c>
@@ -4467,32 +4697,38 @@
       <c r="D16" s="3" t="s">
         <v>384</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E16" s="23" t="s">
+        <v>911</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="G16" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="H16" s="3" t="s">
         <v>358</v>
       </c>
-      <c r="G16" s="22" t="s">
+      <c r="I16" s="22" t="s">
         <v>892</v>
       </c>
-      <c r="H16" s="3" t="s">
+      <c r="J16" s="3" t="s">
         <v>761</v>
       </c>
-      <c r="I16" s="22" t="s">
+      <c r="K16" s="22" t="s">
         <v>776</v>
       </c>
-      <c r="J16" s="22" t="s">
+      <c r="L16" s="22" t="s">
         <v>819</v>
       </c>
-      <c r="K16" s="22" t="s">
+      <c r="M16" s="22" t="s">
         <v>862</v>
       </c>
-      <c r="L16" s="22" t="s">
+      <c r="N16" s="22" t="s">
         <v>891</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>689</v>
       </c>
@@ -4505,30 +4741,36 @@
       <c r="D17" s="3" t="s">
         <v>384</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E17" s="23" t="s">
+        <v>912</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="G17" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="H17" s="3" t="s">
         <v>358</v>
       </c>
-      <c r="G17" s="22" t="s">
+      <c r="I17" s="22" t="s">
         <v>732</v>
       </c>
-      <c r="H17" s="3" t="s">
+      <c r="J17" s="3" t="s">
         <v>761</v>
       </c>
-      <c r="I17" s="22" t="s">
+      <c r="K17" s="22" t="s">
         <v>777</v>
       </c>
-      <c r="J17" s="22" t="s">
+      <c r="L17" s="22" t="s">
         <v>820</v>
       </c>
-      <c r="K17" s="22" t="s">
+      <c r="M17" s="22" t="s">
         <v>863</v>
       </c>
-      <c r="L17" s="23"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N17" s="23"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>690</v>
       </c>
@@ -4541,30 +4783,36 @@
       <c r="D18" s="3" t="s">
         <v>384</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="E18" s="23" t="s">
+        <v>913</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="G18" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F18" s="3" t="s">
+      <c r="H18" s="3" t="s">
         <v>358</v>
       </c>
-      <c r="G18" s="22" t="s">
+      <c r="I18" s="22" t="s">
         <v>733</v>
       </c>
-      <c r="H18" s="3" t="s">
+      <c r="J18" s="3" t="s">
         <v>761</v>
       </c>
-      <c r="I18" s="22" t="s">
+      <c r="K18" s="22" t="s">
         <v>778</v>
       </c>
-      <c r="J18" s="22" t="s">
+      <c r="L18" s="22" t="s">
         <v>821</v>
       </c>
-      <c r="K18" s="22" t="s">
+      <c r="M18" s="22" t="s">
         <v>864</v>
       </c>
-      <c r="L18" s="23"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N18" s="23"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>691</v>
       </c>
@@ -4577,32 +4825,38 @@
       <c r="D19" s="3" t="s">
         <v>384</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="E19" s="23" t="s">
+        <v>914</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="G19" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F19" s="3" t="s">
+      <c r="H19" s="3" t="s">
         <v>358</v>
       </c>
-      <c r="G19" s="22" t="s">
+      <c r="I19" s="22" t="s">
         <v>893</v>
       </c>
-      <c r="H19" s="3" t="s">
+      <c r="J19" s="3" t="s">
         <v>761</v>
       </c>
-      <c r="I19" s="22" t="s">
+      <c r="K19" s="22" t="s">
         <v>776</v>
       </c>
-      <c r="J19" s="22" t="s">
+      <c r="L19" s="22" t="s">
         <v>819</v>
       </c>
-      <c r="K19" s="22" t="s">
+      <c r="M19" s="22" t="s">
         <v>862</v>
       </c>
-      <c r="L19" s="22" t="s">
+      <c r="N19" s="22" t="s">
         <v>894</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>692</v>
       </c>
@@ -4615,30 +4869,36 @@
       <c r="D20" s="3" t="s">
         <v>384</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="E20" s="23" t="s">
+        <v>915</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="G20" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="H20" s="3" t="s">
         <v>358</v>
       </c>
-      <c r="G20" s="22" t="s">
+      <c r="I20" s="22" t="s">
         <v>734</v>
       </c>
-      <c r="H20" s="3" t="s">
+      <c r="J20" s="3" t="s">
         <v>761</v>
       </c>
-      <c r="I20" s="22" t="s">
+      <c r="K20" s="22" t="s">
         <v>779</v>
       </c>
-      <c r="J20" s="22" t="s">
+      <c r="L20" s="22" t="s">
         <v>822</v>
       </c>
-      <c r="K20" s="22" t="s">
+      <c r="M20" s="22" t="s">
         <v>865</v>
       </c>
-      <c r="L20" s="23"/>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N20" s="23"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>693</v>
       </c>
@@ -4651,30 +4911,36 @@
       <c r="D21" s="3" t="s">
         <v>384</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="E21" s="23" t="s">
+        <v>916</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="G21" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F21" s="3" t="s">
+      <c r="H21" s="3" t="s">
         <v>358</v>
       </c>
-      <c r="G21" s="22" t="s">
+      <c r="I21" s="22" t="s">
         <v>735</v>
       </c>
-      <c r="H21" s="3" t="s">
+      <c r="J21" s="3" t="s">
         <v>761</v>
       </c>
-      <c r="I21" s="22" t="s">
+      <c r="K21" s="22" t="s">
         <v>780</v>
       </c>
-      <c r="J21" s="22" t="s">
+      <c r="L21" s="22" t="s">
         <v>823</v>
       </c>
-      <c r="K21" s="22" t="s">
+      <c r="M21" s="22" t="s">
         <v>866</v>
       </c>
-      <c r="L21" s="23"/>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N21" s="23"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>694</v>
       </c>
@@ -4687,30 +4953,36 @@
       <c r="D22" s="3" t="s">
         <v>384</v>
       </c>
-      <c r="E22" s="3" t="s">
+      <c r="E22" s="23" t="s">
+        <v>917</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="G22" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F22" s="3" t="s">
+      <c r="H22" s="3" t="s">
         <v>358</v>
       </c>
-      <c r="G22" s="22" t="s">
+      <c r="I22" s="22" t="s">
         <v>747</v>
       </c>
-      <c r="H22" s="3" t="s">
+      <c r="J22" s="3" t="s">
         <v>761</v>
       </c>
-      <c r="I22" s="22" t="s">
+      <c r="K22" s="22" t="s">
         <v>781</v>
       </c>
-      <c r="J22" s="22" t="s">
+      <c r="L22" s="22" t="s">
         <v>824</v>
       </c>
-      <c r="K22" s="22" t="s">
+      <c r="M22" s="22" t="s">
         <v>867</v>
       </c>
-      <c r="L22" s="23"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N22" s="23"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>695</v>
       </c>
@@ -4723,30 +4995,36 @@
       <c r="D23" s="3" t="s">
         <v>384</v>
       </c>
-      <c r="E23" s="3" t="s">
+      <c r="E23" s="23" t="s">
+        <v>918</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="G23" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F23" s="3" t="s">
+      <c r="H23" s="3" t="s">
         <v>358</v>
       </c>
-      <c r="G23" s="22" t="s">
+      <c r="I23" s="22" t="s">
         <v>748</v>
       </c>
-      <c r="H23" s="3" t="s">
+      <c r="J23" s="3" t="s">
         <v>761</v>
       </c>
-      <c r="I23" s="22" t="s">
+      <c r="K23" s="22" t="s">
         <v>782</v>
       </c>
-      <c r="J23" s="22" t="s">
+      <c r="L23" s="22" t="s">
         <v>825</v>
       </c>
-      <c r="K23" s="22" t="s">
+      <c r="M23" s="22" t="s">
         <v>868</v>
       </c>
-      <c r="L23" s="23"/>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N23" s="23"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>696</v>
       </c>
@@ -4759,30 +5037,36 @@
       <c r="D24" s="3" t="s">
         <v>384</v>
       </c>
-      <c r="E24" s="3" t="s">
+      <c r="E24" s="23" t="s">
+        <v>919</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="G24" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F24" s="3" t="s">
+      <c r="H24" s="3" t="s">
         <v>358</v>
       </c>
-      <c r="G24" s="22" t="s">
+      <c r="I24" s="22" t="s">
         <v>749</v>
       </c>
-      <c r="H24" s="3" t="s">
+      <c r="J24" s="3" t="s">
         <v>761</v>
       </c>
-      <c r="I24" s="22" t="s">
+      <c r="K24" s="22" t="s">
         <v>783</v>
       </c>
-      <c r="J24" s="22" t="s">
+      <c r="L24" s="22" t="s">
         <v>826</v>
       </c>
-      <c r="K24" s="22" t="s">
+      <c r="M24" s="22" t="s">
         <v>869</v>
       </c>
-      <c r="L24" s="23"/>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N24" s="23"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>697</v>
       </c>
@@ -4795,30 +5079,36 @@
       <c r="D25" s="3" t="s">
         <v>384</v>
       </c>
-      <c r="E25" s="3" t="s">
+      <c r="E25" s="23" t="s">
+        <v>920</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="G25" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F25" s="3" t="s">
+      <c r="H25" s="3" t="s">
         <v>358</v>
       </c>
-      <c r="G25" s="22" t="s">
+      <c r="I25" s="22" t="s">
         <v>750</v>
       </c>
-      <c r="H25" s="3" t="s">
+      <c r="J25" s="3" t="s">
         <v>761</v>
       </c>
-      <c r="I25" s="22" t="s">
+      <c r="K25" s="22" t="s">
         <v>784</v>
       </c>
-      <c r="J25" s="22" t="s">
+      <c r="L25" s="22" t="s">
         <v>827</v>
       </c>
-      <c r="K25" s="22" t="s">
+      <c r="M25" s="22" t="s">
         <v>870</v>
       </c>
-      <c r="L25" s="23"/>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N25" s="23"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>698</v>
       </c>
@@ -4831,30 +5121,36 @@
       <c r="D26" s="3" t="s">
         <v>384</v>
       </c>
-      <c r="E26" s="3" t="s">
+      <c r="E26" s="23" t="s">
+        <v>921</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="G26" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F26" s="3" t="s">
+      <c r="H26" s="3" t="s">
         <v>358</v>
       </c>
-      <c r="G26" s="22" t="s">
+      <c r="I26" s="22" t="s">
         <v>736</v>
       </c>
-      <c r="H26" s="3" t="s">
+      <c r="J26" s="3" t="s">
         <v>761</v>
       </c>
-      <c r="I26" s="22" t="s">
+      <c r="K26" s="22" t="s">
         <v>785</v>
       </c>
-      <c r="J26" s="22" t="s">
+      <c r="L26" s="22" t="s">
         <v>828</v>
       </c>
-      <c r="K26" s="22" t="s">
+      <c r="M26" s="22" t="s">
         <v>871</v>
       </c>
-      <c r="L26" s="23"/>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N26" s="23"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>699</v>
       </c>
@@ -4867,30 +5163,36 @@
       <c r="D27" s="3" t="s">
         <v>384</v>
       </c>
-      <c r="E27" s="3" t="s">
+      <c r="E27" s="23" t="s">
+        <v>922</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="G27" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F27" s="3" t="s">
+      <c r="H27" s="3" t="s">
         <v>358</v>
       </c>
-      <c r="G27" s="22" t="s">
+      <c r="I27" s="22" t="s">
         <v>737</v>
       </c>
-      <c r="H27" s="3" t="s">
+      <c r="J27" s="3" t="s">
         <v>761</v>
       </c>
-      <c r="I27" s="22" t="s">
+      <c r="K27" s="22" t="s">
         <v>786</v>
       </c>
-      <c r="J27" s="22" t="s">
+      <c r="L27" s="22" t="s">
         <v>829</v>
       </c>
-      <c r="K27" s="22" t="s">
+      <c r="M27" s="22" t="s">
         <v>872</v>
       </c>
-      <c r="L27" s="23"/>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N27" s="23"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>700</v>
       </c>
@@ -4903,30 +5205,36 @@
       <c r="D28" s="3" t="s">
         <v>384</v>
       </c>
-      <c r="E28" s="3" t="s">
+      <c r="E28" s="23" t="s">
+        <v>923</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="G28" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F28" s="3" t="s">
+      <c r="H28" s="3" t="s">
         <v>358</v>
       </c>
-      <c r="G28" s="22" t="s">
+      <c r="I28" s="22" t="s">
         <v>738</v>
       </c>
-      <c r="H28" s="3" t="s">
+      <c r="J28" s="3" t="s">
         <v>761</v>
       </c>
-      <c r="I28" s="22" t="s">
+      <c r="K28" s="22" t="s">
         <v>787</v>
       </c>
-      <c r="J28" s="22" t="s">
+      <c r="L28" s="22" t="s">
         <v>830</v>
       </c>
-      <c r="K28" s="22" t="s">
+      <c r="M28" s="22" t="s">
         <v>873</v>
       </c>
-      <c r="L28" s="23"/>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N28" s="23"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>701</v>
       </c>
@@ -4939,30 +5247,36 @@
       <c r="D29" s="3" t="s">
         <v>384</v>
       </c>
-      <c r="E29" s="3" t="s">
+      <c r="E29" s="23" t="s">
+        <v>924</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="G29" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F29" s="3" t="s">
+      <c r="H29" s="3" t="s">
         <v>358</v>
       </c>
-      <c r="G29" s="22" t="s">
+      <c r="I29" s="22" t="s">
         <v>739</v>
       </c>
-      <c r="H29" s="3" t="s">
+      <c r="J29" s="3" t="s">
         <v>761</v>
       </c>
-      <c r="I29" s="22" t="s">
+      <c r="K29" s="22" t="s">
         <v>788</v>
       </c>
-      <c r="J29" s="22" t="s">
+      <c r="L29" s="22" t="s">
         <v>831</v>
       </c>
-      <c r="K29" s="22" t="s">
+      <c r="M29" s="22" t="s">
         <v>874</v>
       </c>
-      <c r="L29" s="23"/>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N29" s="23"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>702</v>
       </c>
@@ -4975,30 +5289,36 @@
       <c r="D30" s="3" t="s">
         <v>384</v>
       </c>
-      <c r="E30" s="3" t="s">
+      <c r="E30" s="23" t="s">
+        <v>925</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="G30" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F30" s="3" t="s">
+      <c r="H30" s="3" t="s">
         <v>358</v>
       </c>
-      <c r="G30" s="22" t="s">
+      <c r="I30" s="22" t="s">
         <v>751</v>
       </c>
-      <c r="H30" s="3" t="s">
+      <c r="J30" s="3" t="s">
         <v>761</v>
       </c>
-      <c r="I30" s="22" t="s">
+      <c r="K30" s="22" t="s">
         <v>789</v>
       </c>
-      <c r="J30" s="22" t="s">
+      <c r="L30" s="22" t="s">
         <v>832</v>
       </c>
-      <c r="K30" s="22" t="s">
+      <c r="M30" s="22" t="s">
         <v>875</v>
       </c>
-      <c r="L30" s="23"/>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N30" s="23"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>703</v>
       </c>
@@ -5011,30 +5331,36 @@
       <c r="D31" s="3" t="s">
         <v>384</v>
       </c>
-      <c r="E31" s="3" t="s">
+      <c r="E31" s="23" t="s">
+        <v>926</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="G31" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F31" s="3" t="s">
+      <c r="H31" s="3" t="s">
         <v>358</v>
       </c>
-      <c r="G31" s="22" t="s">
+      <c r="I31" s="22" t="s">
         <v>752</v>
       </c>
-      <c r="H31" s="3" t="s">
+      <c r="J31" s="3" t="s">
         <v>761</v>
       </c>
-      <c r="I31" s="22" t="s">
+      <c r="K31" s="22" t="s">
         <v>790</v>
       </c>
-      <c r="J31" s="22" t="s">
+      <c r="L31" s="22" t="s">
         <v>833</v>
       </c>
-      <c r="K31" s="22" t="s">
+      <c r="M31" s="22" t="s">
         <v>876</v>
       </c>
-      <c r="L31" s="23"/>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N31" s="23"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>704</v>
       </c>
@@ -5047,30 +5373,36 @@
       <c r="D32" s="3" t="s">
         <v>384</v>
       </c>
-      <c r="E32" s="3" t="s">
+      <c r="E32" s="23" t="s">
+        <v>927</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="G32" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F32" s="3" t="s">
+      <c r="H32" s="3" t="s">
         <v>358</v>
       </c>
-      <c r="G32" s="22" t="s">
+      <c r="I32" s="22" t="s">
         <v>740</v>
       </c>
-      <c r="H32" s="3" t="s">
+      <c r="J32" s="3" t="s">
         <v>761</v>
       </c>
-      <c r="I32" s="22" t="s">
+      <c r="K32" s="22" t="s">
         <v>791</v>
       </c>
-      <c r="J32" s="22" t="s">
+      <c r="L32" s="22" t="s">
         <v>834</v>
       </c>
-      <c r="K32" s="22" t="s">
+      <c r="M32" s="22" t="s">
         <v>877</v>
       </c>
-      <c r="L32" s="23"/>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N32" s="23"/>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>705</v>
       </c>
@@ -5083,30 +5415,36 @@
       <c r="D33" s="3" t="s">
         <v>384</v>
       </c>
-      <c r="E33" s="3" t="s">
+      <c r="E33" s="23" t="s">
+        <v>928</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="G33" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F33" s="3" t="s">
+      <c r="H33" s="3" t="s">
         <v>358</v>
       </c>
-      <c r="G33" s="22" t="s">
+      <c r="I33" s="22" t="s">
         <v>753</v>
       </c>
-      <c r="H33" s="3" t="s">
+      <c r="J33" s="3" t="s">
         <v>761</v>
       </c>
-      <c r="I33" s="22" t="s">
+      <c r="K33" s="22" t="s">
         <v>792</v>
       </c>
-      <c r="J33" s="22" t="s">
+      <c r="L33" s="22" t="s">
         <v>835</v>
       </c>
-      <c r="K33" s="22" t="s">
+      <c r="M33" s="22" t="s">
         <v>878</v>
       </c>
-      <c r="L33" s="23"/>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N33" s="23"/>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>706</v>
       </c>
@@ -5119,30 +5457,36 @@
       <c r="D34" s="3" t="s">
         <v>384</v>
       </c>
-      <c r="E34" s="3" t="s">
+      <c r="E34" s="23" t="s">
+        <v>929</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="G34" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F34" s="3" t="s">
+      <c r="H34" s="3" t="s">
         <v>358</v>
       </c>
-      <c r="G34" s="22" t="s">
+      <c r="I34" s="22" t="s">
         <v>754</v>
       </c>
-      <c r="H34" s="3" t="s">
+      <c r="J34" s="3" t="s">
         <v>761</v>
       </c>
-      <c r="I34" s="22" t="s">
+      <c r="K34" s="22" t="s">
         <v>793</v>
       </c>
-      <c r="J34" s="22" t="s">
+      <c r="L34" s="22" t="s">
         <v>836</v>
       </c>
-      <c r="K34" s="22" t="s">
+      <c r="M34" s="22" t="s">
         <v>879</v>
       </c>
-      <c r="L34" s="23"/>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N34" s="23"/>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>707</v>
       </c>
@@ -5155,30 +5499,36 @@
       <c r="D35" s="3" t="s">
         <v>384</v>
       </c>
-      <c r="E35" s="3" t="s">
+      <c r="E35" s="23" t="s">
+        <v>930</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="G35" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F35" s="3" t="s">
+      <c r="H35" s="3" t="s">
         <v>358</v>
       </c>
-      <c r="G35" s="22" t="s">
+      <c r="I35" s="22" t="s">
         <v>755</v>
       </c>
-      <c r="H35" s="3" t="s">
+      <c r="J35" s="3" t="s">
         <v>761</v>
       </c>
-      <c r="I35" s="22" t="s">
+      <c r="K35" s="22" t="s">
         <v>794</v>
       </c>
-      <c r="J35" s="22" t="s">
+      <c r="L35" s="22" t="s">
         <v>837</v>
       </c>
-      <c r="K35" s="22" t="s">
+      <c r="M35" s="22" t="s">
         <v>880</v>
       </c>
-      <c r="L35" s="23"/>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N35" s="23"/>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>708</v>
       </c>
@@ -5191,30 +5541,36 @@
       <c r="D36" s="3" t="s">
         <v>384</v>
       </c>
-      <c r="E36" s="3" t="s">
+      <c r="E36" s="23" t="s">
+        <v>931</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="G36" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F36" s="3" t="s">
+      <c r="H36" s="3" t="s">
         <v>358</v>
       </c>
-      <c r="G36" s="22" t="s">
+      <c r="I36" s="22" t="s">
         <v>741</v>
       </c>
-      <c r="H36" s="3" t="s">
+      <c r="J36" s="3" t="s">
         <v>761</v>
       </c>
-      <c r="I36" s="22" t="s">
+      <c r="K36" s="22" t="s">
         <v>795</v>
       </c>
-      <c r="J36" s="22" t="s">
+      <c r="L36" s="22" t="s">
         <v>838</v>
       </c>
-      <c r="K36" s="22" t="s">
+      <c r="M36" s="22" t="s">
         <v>881</v>
       </c>
-      <c r="L36" s="23"/>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N36" s="23"/>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>709</v>
       </c>
@@ -5227,30 +5583,36 @@
       <c r="D37" s="3" t="s">
         <v>384</v>
       </c>
-      <c r="E37" s="3" t="s">
+      <c r="E37" s="23" t="s">
+        <v>932</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="G37" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F37" s="3" t="s">
+      <c r="H37" s="3" t="s">
         <v>358</v>
       </c>
-      <c r="G37" s="22" t="s">
+      <c r="I37" s="22" t="s">
         <v>756</v>
       </c>
-      <c r="H37" s="3" t="s">
+      <c r="J37" s="3" t="s">
         <v>761</v>
       </c>
-      <c r="I37" s="22" t="s">
+      <c r="K37" s="22" t="s">
         <v>796</v>
       </c>
-      <c r="J37" s="22" t="s">
+      <c r="L37" s="22" t="s">
         <v>839</v>
       </c>
-      <c r="K37" s="22" t="s">
+      <c r="M37" s="22" t="s">
         <v>882</v>
       </c>
-      <c r="L37" s="23"/>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N37" s="23"/>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>710</v>
       </c>
@@ -5263,30 +5625,36 @@
       <c r="D38" s="3" t="s">
         <v>384</v>
       </c>
-      <c r="E38" s="3" t="s">
+      <c r="E38" s="23" t="s">
+        <v>933</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="G38" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F38" s="3" t="s">
+      <c r="H38" s="3" t="s">
         <v>358</v>
       </c>
-      <c r="G38" s="22" t="s">
+      <c r="I38" s="22" t="s">
         <v>757</v>
       </c>
-      <c r="H38" s="3" t="s">
+      <c r="J38" s="3" t="s">
         <v>761</v>
       </c>
-      <c r="I38" s="22" t="s">
+      <c r="K38" s="22" t="s">
         <v>797</v>
       </c>
-      <c r="J38" s="22" t="s">
+      <c r="L38" s="22" t="s">
         <v>840</v>
       </c>
-      <c r="K38" s="22" t="s">
+      <c r="M38" s="22" t="s">
         <v>883</v>
       </c>
-      <c r="L38" s="23"/>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N38" s="23"/>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>711</v>
       </c>
@@ -5299,30 +5667,36 @@
       <c r="D39" s="3" t="s">
         <v>384</v>
       </c>
-      <c r="E39" s="3" t="s">
+      <c r="E39" s="23" t="s">
+        <v>934</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="G39" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F39" s="3" t="s">
+      <c r="H39" s="3" t="s">
         <v>358</v>
       </c>
-      <c r="G39" s="22" t="s">
+      <c r="I39" s="22" t="s">
         <v>742</v>
       </c>
-      <c r="H39" s="3" t="s">
+      <c r="J39" s="3" t="s">
         <v>761</v>
       </c>
-      <c r="I39" s="22" t="s">
+      <c r="K39" s="22" t="s">
         <v>798</v>
       </c>
-      <c r="J39" s="22" t="s">
+      <c r="L39" s="22" t="s">
         <v>841</v>
       </c>
-      <c r="K39" s="22" t="s">
+      <c r="M39" s="22" t="s">
         <v>884</v>
       </c>
-      <c r="L39" s="23"/>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N39" s="23"/>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>712</v>
       </c>
@@ -5335,30 +5709,36 @@
       <c r="D40" s="3" t="s">
         <v>384</v>
       </c>
-      <c r="E40" s="3" t="s">
+      <c r="E40" s="23" t="s">
+        <v>931</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="G40" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F40" s="3" t="s">
+      <c r="H40" s="3" t="s">
         <v>358</v>
       </c>
-      <c r="G40" s="22" t="s">
+      <c r="I40" s="22" t="s">
         <v>741</v>
       </c>
-      <c r="H40" s="3" t="s">
+      <c r="J40" s="3" t="s">
         <v>761</v>
       </c>
-      <c r="I40" s="22" t="s">
+      <c r="K40" s="22" t="s">
         <v>795</v>
       </c>
-      <c r="J40" s="22" t="s">
+      <c r="L40" s="22" t="s">
         <v>838</v>
       </c>
-      <c r="K40" s="22" t="s">
+      <c r="M40" s="22" t="s">
         <v>881</v>
       </c>
-      <c r="L40" s="23"/>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N40" s="23"/>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>713</v>
       </c>
@@ -5371,30 +5751,36 @@
       <c r="D41" s="3" t="s">
         <v>384</v>
       </c>
-      <c r="E41" s="3" t="s">
+      <c r="E41" s="23" t="s">
+        <v>935</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="G41" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F41" s="3" t="s">
+      <c r="H41" s="3" t="s">
         <v>358</v>
       </c>
-      <c r="G41" s="22" t="s">
+      <c r="I41" s="22" t="s">
         <v>743</v>
       </c>
-      <c r="H41" s="3" t="s">
+      <c r="J41" s="3" t="s">
         <v>761</v>
       </c>
-      <c r="I41" s="22" t="s">
+      <c r="K41" s="22" t="s">
         <v>799</v>
       </c>
-      <c r="J41" s="22" t="s">
+      <c r="L41" s="22" t="s">
         <v>842</v>
       </c>
-      <c r="K41" s="22" t="s">
+      <c r="M41" s="22" t="s">
         <v>885</v>
       </c>
-      <c r="L41" s="23"/>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N41" s="23"/>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>714</v>
       </c>
@@ -5407,30 +5793,36 @@
       <c r="D42" s="3" t="s">
         <v>384</v>
       </c>
-      <c r="E42" s="3" t="s">
+      <c r="E42" s="23" t="s">
+        <v>936</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="G42" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F42" s="3" t="s">
+      <c r="H42" s="3" t="s">
         <v>358</v>
       </c>
-      <c r="G42" s="22" t="s">
+      <c r="I42" s="22" t="s">
         <v>758</v>
       </c>
-      <c r="H42" s="3" t="s">
+      <c r="J42" s="3" t="s">
         <v>761</v>
       </c>
-      <c r="I42" s="22" t="s">
+      <c r="K42" s="22" t="s">
         <v>800</v>
       </c>
-      <c r="J42" s="22" t="s">
+      <c r="L42" s="22" t="s">
         <v>843</v>
       </c>
-      <c r="K42" s="22" t="s">
+      <c r="M42" s="22" t="s">
         <v>886</v>
       </c>
-      <c r="L42" s="23"/>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N42" s="23"/>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>715</v>
       </c>
@@ -5443,30 +5835,36 @@
       <c r="D43" s="3" t="s">
         <v>384</v>
       </c>
-      <c r="E43" s="3" t="s">
+      <c r="E43" s="23" t="s">
+        <v>937</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="G43" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F43" s="3" t="s">
+      <c r="H43" s="3" t="s">
         <v>358</v>
       </c>
-      <c r="G43" s="22" t="s">
+      <c r="I43" s="22" t="s">
         <v>744</v>
       </c>
-      <c r="H43" s="3" t="s">
+      <c r="J43" s="3" t="s">
         <v>761</v>
       </c>
-      <c r="I43" s="22" t="s">
+      <c r="K43" s="22" t="s">
         <v>801</v>
       </c>
-      <c r="J43" s="22" t="s">
+      <c r="L43" s="22" t="s">
         <v>844</v>
       </c>
-      <c r="K43" s="22" t="s">
+      <c r="M43" s="22" t="s">
         <v>887</v>
       </c>
-      <c r="L43" s="23"/>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N43" s="23"/>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>716</v>
       </c>
@@ -5479,30 +5877,36 @@
       <c r="D44" s="3" t="s">
         <v>384</v>
       </c>
-      <c r="E44" s="3" t="s">
+      <c r="E44" s="23" t="s">
+        <v>938</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="G44" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F44" s="3" t="s">
+      <c r="H44" s="3" t="s">
         <v>358</v>
       </c>
-      <c r="G44" s="22" t="s">
+      <c r="I44" s="22" t="s">
         <v>759</v>
       </c>
-      <c r="H44" s="3" t="s">
+      <c r="J44" s="3" t="s">
         <v>761</v>
       </c>
-      <c r="I44" s="22" t="s">
+      <c r="K44" s="22" t="s">
         <v>802</v>
       </c>
-      <c r="J44" s="22" t="s">
+      <c r="L44" s="22" t="s">
         <v>845</v>
       </c>
-      <c r="K44" s="22" t="s">
+      <c r="M44" s="22" t="s">
         <v>888</v>
       </c>
-      <c r="L44" s="23"/>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N44" s="23"/>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>717</v>
       </c>
@@ -5515,30 +5919,36 @@
       <c r="D45" s="3" t="s">
         <v>384</v>
       </c>
-      <c r="E45" s="3" t="s">
+      <c r="E45" s="23" t="s">
+        <v>939</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="G45" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F45" s="3" t="s">
+      <c r="H45" s="3" t="s">
         <v>358</v>
       </c>
-      <c r="G45" s="22" t="s">
+      <c r="I45" s="22" t="s">
         <v>760</v>
       </c>
-      <c r="H45" s="3" t="s">
+      <c r="J45" s="3" t="s">
         <v>761</v>
       </c>
-      <c r="I45" s="22" t="s">
+      <c r="K45" s="22" t="s">
         <v>803</v>
       </c>
-      <c r="J45" s="22" t="s">
+      <c r="L45" s="22" t="s">
         <v>846</v>
       </c>
-      <c r="K45" s="22" t="s">
+      <c r="M45" s="22" t="s">
         <v>889</v>
       </c>
-      <c r="L45" s="23"/>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N45" s="23"/>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>718</v>
       </c>
@@ -5551,28 +5961,34 @@
       <c r="D46" s="3" t="s">
         <v>384</v>
       </c>
-      <c r="E46" s="3" t="s">
+      <c r="E46" s="23" t="s">
+        <v>940</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="G46" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F46" s="3" t="s">
+      <c r="H46" s="3" t="s">
         <v>358</v>
       </c>
-      <c r="G46" s="22" t="s">
+      <c r="I46" s="22" t="s">
         <v>745</v>
       </c>
-      <c r="H46" s="3" t="s">
+      <c r="J46" s="3" t="s">
         <v>761</v>
       </c>
-      <c r="I46" s="22" t="s">
+      <c r="K46" s="22" t="s">
         <v>804</v>
       </c>
-      <c r="J46" s="22" t="s">
+      <c r="L46" s="22" t="s">
         <v>847</v>
       </c>
-      <c r="K46" s="22" t="s">
+      <c r="M46" s="22" t="s">
         <v>890</v>
       </c>
-      <c r="L46" s="23"/>
+      <c r="N46" s="23"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
@@ -5594,7 +6010,7 @@
   </conditionalFormatting>
   <dataValidations count="2">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid entry" error="Please choose a value from the dropdown list" prompt="Please choose a value from the dropdown list" sqref="B1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid value" error="Please select a value from the drop-down list" prompt="Please select a header from the drop-down list" sqref="F1"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid value" error="Please select a value from the drop-down list" prompt="Please select a header from the drop-down list" sqref="H1"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5606,13 +6022,13 @@
           <x14:formula1>
             <xm:f>'CV values'!$B$2:$B$21</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:D1048576</xm:sqref>
+          <xm:sqref>D2:D1048576 F2:F1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid entry" error="Please choose a value from the dropdown list" prompt="Please choose a value from the dropdown list">
           <x14:formula1>
             <xm:f>'CV values'!$C$2:$C$15</xm:f>
           </x14:formula1>
-          <xm:sqref>E2:E1048576</xm:sqref>
+          <xm:sqref>G2:G1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid entry" error="Please choose a value from the dropdown list" prompt="Please choose a value from the dropdown list">
           <x14:formula1>
@@ -5624,25 +6040,25 @@
           <x14:formula1>
             <xm:f>'Select-a-header values'!$A$1:$A$7</xm:f>
           </x14:formula1>
-          <xm:sqref>G1</xm:sqref>
+          <xm:sqref>I1</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid value" error="Please select a value from the drop-down list" prompt="Please select a header from the drop-down list">
           <x14:formula1>
             <xm:f>'CV values'!$D$2:$D$60</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F1048576</xm:sqref>
+          <xm:sqref>H2:H1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
           <x14:formula1>
             <xm:f>'Select-a-header values'!$C$1:$C$185</xm:f>
           </x14:formula1>
-          <xm:sqref>H1</xm:sqref>
+          <xm:sqref>J1</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
           <x14:formula1>
             <xm:f>'Select-a-header values'!$D$1:$D$6</xm:f>
           </x14:formula1>
-          <xm:sqref>I1</xm:sqref>
+          <xm:sqref>K1</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Fixed some file names that had changed, based on File Match tool report
</commit_message>
<xml_diff>
--- a/course_catalogs/OLR/xls_standard_input_UCSD-course-catalogs.xlsx
+++ b/course_catalogs/OLR/xls_standard_input_UCSD-course-catalogs.xlsx
@@ -133,7 +133,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1228" uniqueCount="941">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1226" uniqueCount="940">
   <si>
     <t>text</t>
   </si>
@@ -2145,9 +2145,6 @@
     <t>UCSDGC_1976-1977.pdf</t>
   </si>
   <si>
-    <t>UCSDGC_1999_2000.pdf</t>
-  </si>
-  <si>
     <t>UCSDGC_1995-1996.pdf</t>
   </si>
   <si>
@@ -2862,9 +2859,6 @@
     <t>UCSDGC_1973-1974.zip</t>
   </si>
   <si>
-    <t>UCSDGC_1967-1968.zip</t>
-  </si>
-  <si>
     <t>UCSDGC_1961-1962.zip</t>
   </si>
   <si>
@@ -2943,9 +2937,6 @@
     <t>UCSDGC_1976-1977.zip</t>
   </si>
   <si>
-    <t>UCSDGC_1999_2000.zip</t>
-  </si>
-  <si>
     <t>UCSDGC_1995-1996.zip</t>
   </si>
   <si>
@@ -2956,6 +2947,12 @@
   </si>
   <si>
     <t>UCSDGC_1990-1991.zip</t>
+  </si>
+  <si>
+    <t>1999_2000_UCSDGC.pdf</t>
+  </si>
+  <si>
+    <t>1999_2000_UCSDGC.zip</t>
   </si>
 </sst>
 </file>
@@ -4031,7 +4028,7 @@
   <dimension ref="A1:N46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4066,10 +4063,10 @@
         <v>3</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="F1" s="15" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="G1" s="15" t="s">
         <v>9</v>
@@ -4110,7 +4107,7 @@
         <v>384</v>
       </c>
       <c r="E2" s="23" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>381</v>
@@ -4122,25 +4119,25 @@
         <v>358</v>
       </c>
       <c r="I2" s="22" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="J2" s="3" t="s">
+        <v>760</v>
+      </c>
+      <c r="K2" s="22" t="s">
         <v>761</v>
       </c>
-      <c r="K2" s="22" t="s">
-        <v>762</v>
-      </c>
       <c r="L2" s="22" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="M2" s="22" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="N2" s="23"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>485</v>
@@ -4152,7 +4149,7 @@
         <v>384</v>
       </c>
       <c r="E3" s="23" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>381</v>
@@ -4164,25 +4161,25 @@
         <v>358</v>
       </c>
       <c r="I3" s="22" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="K3" s="22" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="L3" s="22" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="M3" s="22" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="N3" s="23"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>485</v>
@@ -4194,7 +4191,7 @@
         <v>384</v>
       </c>
       <c r="E4" s="23" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>381</v>
@@ -4206,25 +4203,25 @@
         <v>358</v>
       </c>
       <c r="I4" s="22" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="K4" s="22" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="L4" s="22" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="M4" s="22" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="N4" s="23"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>485</v>
@@ -4236,7 +4233,7 @@
         <v>384</v>
       </c>
       <c r="E5" s="23" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>381</v>
@@ -4248,25 +4245,25 @@
         <v>358</v>
       </c>
       <c r="I5" s="22" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="K5" s="22" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="L5" s="22" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="M5" s="22" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="N5" s="23"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>485</v>
@@ -4278,7 +4275,7 @@
         <v>384</v>
       </c>
       <c r="E6" s="23" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>381</v>
@@ -4290,25 +4287,25 @@
         <v>358</v>
       </c>
       <c r="I6" s="22" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="K6" s="22" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="L6" s="22" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="M6" s="22" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="N6" s="23"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>485</v>
@@ -4320,7 +4317,7 @@
         <v>384</v>
       </c>
       <c r="E7" s="23" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>381</v>
@@ -4332,25 +4329,25 @@
         <v>358</v>
       </c>
       <c r="I7" s="22" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="K7" s="22" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="L7" s="22" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="M7" s="22" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="N7" s="23"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>485</v>
@@ -4362,7 +4359,7 @@
         <v>384</v>
       </c>
       <c r="E8" s="23" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>381</v>
@@ -4374,25 +4371,25 @@
         <v>358</v>
       </c>
       <c r="I8" s="22" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="K8" s="22" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="L8" s="22" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="M8" s="22" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="N8" s="23"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>485</v>
@@ -4404,7 +4401,7 @@
         <v>384</v>
       </c>
       <c r="E9" s="23" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>381</v>
@@ -4416,25 +4413,25 @@
         <v>358</v>
       </c>
       <c r="I9" s="22" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="K9" s="22" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="L9" s="22" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="M9" s="22" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="N9" s="23"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>485</v>
@@ -4446,7 +4443,7 @@
         <v>384</v>
       </c>
       <c r="E10" s="23" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>381</v>
@@ -4458,25 +4455,25 @@
         <v>358</v>
       </c>
       <c r="I10" s="22" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="K10" s="22" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="L10" s="22" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="M10" s="22" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="N10" s="23"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>485</v>
@@ -4488,7 +4485,7 @@
         <v>384</v>
       </c>
       <c r="E11" s="23" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>381</v>
@@ -4500,25 +4497,25 @@
         <v>358</v>
       </c>
       <c r="I11" s="22" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="K11" s="22" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="L11" s="22" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="M11" s="22" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="N11" s="23"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>485</v>
@@ -4530,7 +4527,7 @@
         <v>384</v>
       </c>
       <c r="E12" s="23" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>381</v>
@@ -4542,25 +4539,25 @@
         <v>358</v>
       </c>
       <c r="I12" s="22" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="K12" s="22" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="L12" s="22" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="M12" s="22" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="N12" s="23"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>485</v>
@@ -4572,7 +4569,7 @@
         <v>384</v>
       </c>
       <c r="E13" s="23" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>381</v>
@@ -4584,25 +4581,25 @@
         <v>358</v>
       </c>
       <c r="I13" s="22" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="K13" s="22" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="L13" s="22" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="M13" s="22" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="N13" s="23"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>485</v>
@@ -4613,12 +4610,7 @@
       <c r="D14" s="3" t="s">
         <v>384</v>
       </c>
-      <c r="E14" s="23" t="s">
-        <v>909</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>381</v>
-      </c>
+      <c r="E14" s="23"/>
       <c r="G14" s="3" t="s">
         <v>0</v>
       </c>
@@ -4626,25 +4618,25 @@
         <v>358</v>
       </c>
       <c r="I14" s="22" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="K14" s="22" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="L14" s="22" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="M14" s="22" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="N14" s="23"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>485</v>
@@ -4656,7 +4648,7 @@
         <v>384</v>
       </c>
       <c r="E15" s="23" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>381</v>
@@ -4668,25 +4660,25 @@
         <v>358</v>
       </c>
       <c r="I15" s="22" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="K15" s="22" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="L15" s="22" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="M15" s="22" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="N15" s="23"/>
     </row>
     <row r="16" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>485</v>
@@ -4698,7 +4690,7 @@
         <v>384</v>
       </c>
       <c r="E16" s="23" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>381</v>
@@ -4710,27 +4702,27 @@
         <v>358</v>
       </c>
       <c r="I16" s="22" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="K16" s="22" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="L16" s="22" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="M16" s="22" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="N16" s="22" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>485</v>
@@ -4742,7 +4734,7 @@
         <v>384</v>
       </c>
       <c r="E17" s="23" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="F17" s="3" t="s">
         <v>381</v>
@@ -4754,25 +4746,25 @@
         <v>358</v>
       </c>
       <c r="I17" s="22" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="K17" s="22" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="L17" s="22" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="M17" s="22" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="N17" s="23"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>485</v>
@@ -4784,7 +4776,7 @@
         <v>384</v>
       </c>
       <c r="E18" s="23" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>381</v>
@@ -4796,25 +4788,25 @@
         <v>358</v>
       </c>
       <c r="I18" s="22" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="K18" s="22" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="L18" s="22" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="M18" s="22" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="N18" s="23"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>485</v>
@@ -4826,7 +4818,7 @@
         <v>384</v>
       </c>
       <c r="E19" s="23" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>381</v>
@@ -4838,27 +4830,27 @@
         <v>358</v>
       </c>
       <c r="I19" s="22" t="s">
+        <v>892</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>760</v>
+      </c>
+      <c r="K19" s="22" t="s">
+        <v>775</v>
+      </c>
+      <c r="L19" s="22" t="s">
+        <v>818</v>
+      </c>
+      <c r="M19" s="22" t="s">
+        <v>861</v>
+      </c>
+      <c r="N19" s="22" t="s">
         <v>893</v>
-      </c>
-      <c r="J19" s="3" t="s">
-        <v>761</v>
-      </c>
-      <c r="K19" s="22" t="s">
-        <v>776</v>
-      </c>
-      <c r="L19" s="22" t="s">
-        <v>819</v>
-      </c>
-      <c r="M19" s="22" t="s">
-        <v>862</v>
-      </c>
-      <c r="N19" s="22" t="s">
-        <v>894</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>485</v>
@@ -4870,7 +4862,7 @@
         <v>384</v>
       </c>
       <c r="E20" s="23" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>381</v>
@@ -4882,25 +4874,25 @@
         <v>358</v>
       </c>
       <c r="I20" s="22" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="K20" s="22" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="L20" s="22" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="M20" s="22" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="N20" s="23"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>485</v>
@@ -4912,7 +4904,7 @@
         <v>384</v>
       </c>
       <c r="E21" s="23" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>381</v>
@@ -4924,25 +4916,25 @@
         <v>358</v>
       </c>
       <c r="I21" s="22" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="K21" s="22" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="L21" s="22" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="M21" s="22" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="N21" s="23"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>485</v>
@@ -4954,7 +4946,7 @@
         <v>384</v>
       </c>
       <c r="E22" s="23" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>381</v>
@@ -4966,25 +4958,25 @@
         <v>358</v>
       </c>
       <c r="I22" s="22" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="K22" s="22" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="L22" s="22" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="M22" s="22" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="N22" s="23"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>485</v>
@@ -4996,7 +4988,7 @@
         <v>384</v>
       </c>
       <c r="E23" s="23" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
       <c r="F23" s="3" t="s">
         <v>381</v>
@@ -5008,25 +5000,25 @@
         <v>358</v>
       </c>
       <c r="I23" s="22" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="K23" s="22" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="L23" s="22" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="M23" s="22" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="N23" s="23"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>485</v>
@@ -5038,7 +5030,7 @@
         <v>384</v>
       </c>
       <c r="E24" s="23" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
       <c r="F24" s="3" t="s">
         <v>381</v>
@@ -5050,25 +5042,25 @@
         <v>358</v>
       </c>
       <c r="I24" s="22" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="K24" s="22" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="L24" s="22" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="M24" s="22" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="N24" s="23"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>485</v>
@@ -5080,7 +5072,7 @@
         <v>384</v>
       </c>
       <c r="E25" s="23" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
       <c r="F25" s="3" t="s">
         <v>381</v>
@@ -5092,25 +5084,25 @@
         <v>358</v>
       </c>
       <c r="I25" s="22" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="K25" s="22" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="L25" s="22" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="M25" s="22" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="N25" s="23"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>485</v>
@@ -5122,7 +5114,7 @@
         <v>384</v>
       </c>
       <c r="E26" s="23" t="s">
-        <v>921</v>
+        <v>919</v>
       </c>
       <c r="F26" s="3" t="s">
         <v>381</v>
@@ -5134,25 +5126,25 @@
         <v>358</v>
       </c>
       <c r="I26" s="22" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="K26" s="22" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="L26" s="22" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="M26" s="22" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="N26" s="23"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>485</v>
@@ -5164,7 +5156,7 @@
         <v>384</v>
       </c>
       <c r="E27" s="23" t="s">
-        <v>922</v>
+        <v>920</v>
       </c>
       <c r="F27" s="3" t="s">
         <v>381</v>
@@ -5176,25 +5168,25 @@
         <v>358</v>
       </c>
       <c r="I27" s="22" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="K27" s="22" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="L27" s="22" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="M27" s="22" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="N27" s="23"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>485</v>
@@ -5206,7 +5198,7 @@
         <v>384</v>
       </c>
       <c r="E28" s="23" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
       <c r="F28" s="3" t="s">
         <v>381</v>
@@ -5218,25 +5210,25 @@
         <v>358</v>
       </c>
       <c r="I28" s="22" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="K28" s="22" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="L28" s="22" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="M28" s="22" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="N28" s="23"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>485</v>
@@ -5248,7 +5240,7 @@
         <v>384</v>
       </c>
       <c r="E29" s="23" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
       <c r="F29" s="3" t="s">
         <v>381</v>
@@ -5260,25 +5252,25 @@
         <v>358</v>
       </c>
       <c r="I29" s="22" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="K29" s="22" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="L29" s="22" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="M29" s="22" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="N29" s="23"/>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>485</v>
@@ -5290,7 +5282,7 @@
         <v>384</v>
       </c>
       <c r="E30" s="23" t="s">
-        <v>925</v>
+        <v>923</v>
       </c>
       <c r="F30" s="3" t="s">
         <v>381</v>
@@ -5302,25 +5294,25 @@
         <v>358</v>
       </c>
       <c r="I30" s="22" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="J30" s="3" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="K30" s="22" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="L30" s="22" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="M30" s="22" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="N30" s="23"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>485</v>
@@ -5332,7 +5324,7 @@
         <v>384</v>
       </c>
       <c r="E31" s="23" t="s">
-        <v>926</v>
+        <v>924</v>
       </c>
       <c r="F31" s="3" t="s">
         <v>381</v>
@@ -5344,25 +5336,25 @@
         <v>358</v>
       </c>
       <c r="I31" s="22" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="K31" s="22" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="L31" s="22" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="M31" s="22" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="N31" s="23"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>485</v>
@@ -5374,7 +5366,7 @@
         <v>384</v>
       </c>
       <c r="E32" s="23" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
       <c r="F32" s="3" t="s">
         <v>381</v>
@@ -5386,25 +5378,25 @@
         <v>358</v>
       </c>
       <c r="I32" s="22" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="J32" s="3" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="K32" s="22" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="L32" s="22" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="M32" s="22" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="N32" s="23"/>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>485</v>
@@ -5416,7 +5408,7 @@
         <v>384</v>
       </c>
       <c r="E33" s="23" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="F33" s="3" t="s">
         <v>381</v>
@@ -5428,25 +5420,25 @@
         <v>358</v>
       </c>
       <c r="I33" s="22" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="J33" s="3" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="K33" s="22" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="L33" s="22" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="M33" s="22" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="N33" s="23"/>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>485</v>
@@ -5458,7 +5450,7 @@
         <v>384</v>
       </c>
       <c r="E34" s="23" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
       <c r="F34" s="3" t="s">
         <v>381</v>
@@ -5470,25 +5462,25 @@
         <v>358</v>
       </c>
       <c r="I34" s="22" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="J34" s="3" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="K34" s="22" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="L34" s="22" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="M34" s="22" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="N34" s="23"/>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>485</v>
@@ -5500,7 +5492,7 @@
         <v>384</v>
       </c>
       <c r="E35" s="23" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
       <c r="F35" s="3" t="s">
         <v>381</v>
@@ -5512,25 +5504,25 @@
         <v>358</v>
       </c>
       <c r="I35" s="22" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="J35" s="3" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="K35" s="22" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="L35" s="22" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="M35" s="22" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="N35" s="23"/>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>485</v>
@@ -5542,7 +5534,7 @@
         <v>384</v>
       </c>
       <c r="E36" s="23" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="F36" s="3" t="s">
         <v>381</v>
@@ -5554,25 +5546,25 @@
         <v>358</v>
       </c>
       <c r="I36" s="22" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="J36" s="3" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="K36" s="22" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="L36" s="22" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="M36" s="22" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="N36" s="23"/>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>485</v>
@@ -5584,7 +5576,7 @@
         <v>384</v>
       </c>
       <c r="E37" s="23" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
       <c r="F37" s="3" t="s">
         <v>381</v>
@@ -5596,25 +5588,25 @@
         <v>358</v>
       </c>
       <c r="I37" s="22" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="J37" s="3" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="K37" s="22" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="L37" s="22" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="M37" s="22" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="N37" s="23"/>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>485</v>
@@ -5626,7 +5618,7 @@
         <v>384</v>
       </c>
       <c r="E38" s="23" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="F38" s="3" t="s">
         <v>381</v>
@@ -5638,25 +5630,25 @@
         <v>358</v>
       </c>
       <c r="I38" s="22" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="J38" s="3" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="K38" s="22" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="L38" s="22" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="M38" s="22" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="N38" s="23"/>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>485</v>
@@ -5668,7 +5660,7 @@
         <v>384</v>
       </c>
       <c r="E39" s="23" t="s">
-        <v>934</v>
+        <v>932</v>
       </c>
       <c r="F39" s="3" t="s">
         <v>381</v>
@@ -5680,25 +5672,25 @@
         <v>358</v>
       </c>
       <c r="I39" s="22" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="J39" s="3" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="K39" s="22" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="L39" s="22" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="M39" s="22" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="N39" s="23"/>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>485</v>
@@ -5710,7 +5702,7 @@
         <v>384</v>
       </c>
       <c r="E40" s="23" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="F40" s="3" t="s">
         <v>381</v>
@@ -5722,25 +5714,25 @@
         <v>358</v>
       </c>
       <c r="I40" s="22" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="J40" s="3" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="K40" s="22" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="L40" s="22" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="M40" s="22" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="N40" s="23"/>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>485</v>
@@ -5752,7 +5744,7 @@
         <v>384</v>
       </c>
       <c r="E41" s="23" t="s">
-        <v>935</v>
+        <v>933</v>
       </c>
       <c r="F41" s="3" t="s">
         <v>381</v>
@@ -5764,37 +5756,37 @@
         <v>358</v>
       </c>
       <c r="I41" s="22" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="J41" s="3" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="K41" s="22" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="L41" s="22" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="M41" s="22" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="N41" s="23"/>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>485</v>
       </c>
       <c r="C42" s="23" t="s">
-        <v>670</v>
+        <v>938</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>384</v>
       </c>
       <c r="E42" s="23" t="s">
-        <v>936</v>
+        <v>939</v>
       </c>
       <c r="F42" s="3" t="s">
         <v>381</v>
@@ -5806,37 +5798,37 @@
         <v>358</v>
       </c>
       <c r="I42" s="22" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="J42" s="3" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="K42" s="22" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="L42" s="22" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="M42" s="22" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="N42" s="23"/>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>485</v>
       </c>
       <c r="C43" s="23" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="D43" s="3" t="s">
         <v>384</v>
       </c>
       <c r="E43" s="23" t="s">
-        <v>937</v>
+        <v>934</v>
       </c>
       <c r="F43" s="3" t="s">
         <v>381</v>
@@ -5848,37 +5840,37 @@
         <v>358</v>
       </c>
       <c r="I43" s="22" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="J43" s="3" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="K43" s="22" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="L43" s="22" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="M43" s="22" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="N43" s="23"/>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>485</v>
       </c>
       <c r="C44" s="23" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="D44" s="3" t="s">
         <v>384</v>
       </c>
       <c r="E44" s="23" t="s">
-        <v>938</v>
+        <v>935</v>
       </c>
       <c r="F44" s="3" t="s">
         <v>381</v>
@@ -5890,37 +5882,37 @@
         <v>358</v>
       </c>
       <c r="I44" s="22" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="J44" s="3" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="K44" s="22" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="L44" s="22" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="M44" s="22" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="N44" s="23"/>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>485</v>
       </c>
       <c r="C45" s="23" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="D45" s="3" t="s">
         <v>384</v>
       </c>
       <c r="E45" s="23" t="s">
-        <v>939</v>
+        <v>936</v>
       </c>
       <c r="F45" s="3" t="s">
         <v>381</v>
@@ -5932,37 +5924,37 @@
         <v>358</v>
       </c>
       <c r="I45" s="22" t="s">
+        <v>759</v>
+      </c>
+      <c r="J45" s="3" t="s">
         <v>760</v>
       </c>
-      <c r="J45" s="3" t="s">
-        <v>761</v>
-      </c>
       <c r="K45" s="22" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="L45" s="22" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="M45" s="22" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="N45" s="23"/>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>485</v>
       </c>
       <c r="C46" s="23" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="D46" s="3" t="s">
         <v>384</v>
       </c>
       <c r="E46" s="23" t="s">
-        <v>940</v>
+        <v>937</v>
       </c>
       <c r="F46" s="3" t="s">
         <v>381</v>
@@ -5974,19 +5966,19 @@
         <v>358</v>
       </c>
       <c r="I46" s="22" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="J46" s="3" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="K46" s="22" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="L46" s="22" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="M46" s="22" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="N46" s="23"/>
     </row>

</xml_diff>